<commit_message>
update template report flow meter
</commit_message>
<xml_diff>
--- a/Report/flow.xlsx
+++ b/Report/flow.xlsx
@@ -1390,73 +1390,73 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="1" c:formatCode="hh:mm;@">
-                  <c:v>0</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="2" c:formatCode="hh:mm;@">
-                  <c:v>0</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="3" c:formatCode="hh:mm;@">
-                  <c:v>0</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="4" c:formatCode="hh:mm;@">
-                  <c:v>0</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="5" c:formatCode="hh:mm;@">
-                  <c:v>0</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="6" c:formatCode="hh:mm;@">
-                  <c:v>0</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="7" c:formatCode="hh:mm;@">
-                  <c:v>0</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="8" c:formatCode="hh:mm;@">
-                  <c:v>0</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="9" c:formatCode="hh:mm;@">
-                  <c:v>0</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="10" c:formatCode="hh:mm;@">
-                  <c:v>0</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="11" c:formatCode="hh:mm;@">
-                  <c:v>0</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="12" c:formatCode="hh:mm;@">
-                  <c:v>0</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="13" c:formatCode="hh:mm;@">
-                  <c:v>0</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="14" c:formatCode="hh:mm;@">
-                  <c:v>0</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="15" c:formatCode="hh:mm;@">
-                  <c:v>0</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="16" c:formatCode="hh:mm;@">
-                  <c:v>0</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="17" c:formatCode="hh:mm;@">
-                  <c:v>0</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="18" c:formatCode="hh:mm;@">
-                  <c:v>0</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="19" c:formatCode="hh:mm;@">
-                  <c:v>0</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="20" c:formatCode="hh:mm;@">
-                  <c:v>0</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="21" c:formatCode="hh:mm;@">
-                  <c:v>0</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="22" c:formatCode="hh:mm;@">
-                  <c:v>0</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="23" c:formatCode="hh:mm;@">
-                  <c:v>0</c:v>
+                  <c:v/>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2671,8 +2671,8 @@
   <sheetPr/>
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="6"/>
@@ -2838,9 +2838,9 @@
         <f>A13</f>
         <v/>
       </c>
-      <c r="C13" s="23" t="e">
-        <f>B13+(1/24)</f>
-        <v>#VALUE!</v>
+      <c r="C13" s="23" t="str">
+        <f>IF(B13&lt;&gt;"",B13+(1/24),"")</f>
+        <v/>
       </c>
       <c r="D13" s="24">
         <f>IF(COUNTIFS(RawData!$B$3:$B$6000,"&gt;="&amp;B13,RawData!$B$3:$B$6000,"&lt;"&amp;C13)&gt;0,AVERAGEIFS(RawData!$C$3:$C$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B13,RawData!$B$3:$B$6000,"&lt;"&amp;C13),0)</f>
@@ -2864,13 +2864,13 @@
         <f>A13</f>
         <v/>
       </c>
-      <c r="B14" s="26" t="e">
+      <c r="B14" s="26" t="str">
         <f>C13</f>
-        <v>#VALUE!</v>
+        <v/>
       </c>
-      <c r="C14" s="26" t="e">
-        <f t="shared" ref="C14:C24" si="0">B14+(1/24)</f>
-        <v>#VALUE!</v>
+      <c r="C14" s="23" t="str">
+        <f t="shared" ref="C14:C25" si="0">IF(B14&lt;&gt;"",B14+(1/24),"")</f>
+        <v/>
       </c>
       <c r="D14" s="27">
         <f>IF(COUNTIFS(RawData!$B$3:$B$6000,"&gt;="&amp;B14,RawData!$B$3:$B$6000,"&lt;"&amp;C14)&gt;0,AVERAGEIFS(RawData!$C$3:$C$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B14,RawData!$B$3:$B$6000,"&lt;"&amp;C14),0)</f>
@@ -2891,13 +2891,13 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="2"/>
-      <c r="B15" s="26" t="e">
+      <c r="B15" s="26" t="str">
         <f t="shared" ref="B15:B24" si="3">C14</f>
-        <v>#VALUE!</v>
+        <v/>
       </c>
-      <c r="C15" s="26" t="e">
+      <c r="C15" s="23" t="str">
         <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+        <v/>
       </c>
       <c r="D15" s="27">
         <f>IF(COUNTIFS(RawData!$B$3:$B$6000,"&gt;="&amp;B15,RawData!$B$3:$B$6000,"&lt;"&amp;C15)&gt;0,AVERAGEIFS(RawData!$C$3:$C$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B15,RawData!$B$3:$B$6000,"&lt;"&amp;C15),0)</f>
@@ -2918,13 +2918,13 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="2"/>
-      <c r="B16" s="26" t="e">
+      <c r="B16" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
+        <v/>
       </c>
-      <c r="C16" s="26" t="e">
+      <c r="C16" s="23" t="str">
         <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+        <v/>
       </c>
       <c r="D16" s="27">
         <f>IF(COUNTIFS(RawData!$B$3:$B$6000,"&gt;="&amp;B16,RawData!$B$3:$B$6000,"&lt;"&amp;C16)&gt;0,AVERAGEIFS(RawData!$C$3:$C$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B16,RawData!$B$3:$B$6000,"&lt;"&amp;C16),0)</f>
@@ -2945,13 +2945,13 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="2"/>
-      <c r="B17" s="26" t="e">
+      <c r="B17" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
+        <v/>
       </c>
-      <c r="C17" s="26" t="e">
+      <c r="C17" s="23" t="str">
         <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+        <v/>
       </c>
       <c r="D17" s="27">
         <f>IF(COUNTIFS(RawData!$B$3:$B$6000,"&gt;="&amp;B17,RawData!$B$3:$B$6000,"&lt;"&amp;C17)&gt;0,AVERAGEIFS(RawData!$C$3:$C$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B17,RawData!$B$3:$B$6000,"&lt;"&amp;C17),0)</f>
@@ -2972,13 +2972,13 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="2"/>
-      <c r="B18" s="26" t="e">
+      <c r="B18" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
+        <v/>
       </c>
-      <c r="C18" s="26" t="e">
+      <c r="C18" s="23" t="str">
         <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+        <v/>
       </c>
       <c r="D18" s="27">
         <f>IF(COUNTIFS(RawData!$B$3:$B$6000,"&gt;="&amp;B18,RawData!$B$3:$B$6000,"&lt;"&amp;C18)&gt;0,AVERAGEIFS(RawData!$C$3:$C$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B18,RawData!$B$3:$B$6000,"&lt;"&amp;C18),0)</f>
@@ -2999,13 +2999,13 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="2"/>
-      <c r="B19" s="26" t="e">
+      <c r="B19" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
+        <v/>
       </c>
-      <c r="C19" s="26" t="e">
+      <c r="C19" s="23" t="str">
         <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+        <v/>
       </c>
       <c r="D19" s="27">
         <f>IF(COUNTIFS(RawData!$B$3:$B$6000,"&gt;="&amp;B19,RawData!$B$3:$B$6000,"&lt;"&amp;C19)&gt;0,AVERAGEIFS(RawData!$C$3:$C$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B19,RawData!$B$3:$B$6000,"&lt;"&amp;C19),0)</f>
@@ -3026,13 +3026,13 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="2"/>
-      <c r="B20" s="26" t="e">
+      <c r="B20" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
+        <v/>
       </c>
-      <c r="C20" s="26" t="e">
+      <c r="C20" s="23" t="str">
         <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+        <v/>
       </c>
       <c r="D20" s="27">
         <f>IF(COUNTIFS(RawData!$B$3:$B$6000,"&gt;="&amp;B20,RawData!$B$3:$B$6000,"&lt;"&amp;C20)&gt;0,AVERAGEIFS(RawData!$C$3:$C$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B20,RawData!$B$3:$B$6000,"&lt;"&amp;C20),0)</f>
@@ -3053,13 +3053,13 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="2"/>
-      <c r="B21" s="26" t="e">
+      <c r="B21" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
+        <v/>
       </c>
-      <c r="C21" s="26" t="e">
+      <c r="C21" s="23" t="str">
         <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+        <v/>
       </c>
       <c r="D21" s="27">
         <f>IF(COUNTIFS(RawData!$B$3:$B$6000,"&gt;="&amp;B21,RawData!$B$3:$B$6000,"&lt;"&amp;C21)&gt;0,AVERAGEIFS(RawData!$C$3:$C$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B21,RawData!$B$3:$B$6000,"&lt;"&amp;C21),0)</f>
@@ -3080,13 +3080,13 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="2"/>
-      <c r="B22" s="26" t="e">
+      <c r="B22" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
+        <v/>
       </c>
-      <c r="C22" s="26" t="e">
+      <c r="C22" s="23" t="str">
         <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+        <v/>
       </c>
       <c r="D22" s="27">
         <f>IF(COUNTIFS(RawData!$B$3:$B$6000,"&gt;="&amp;B22,RawData!$B$3:$B$6000,"&lt;"&amp;C22)&gt;0,AVERAGEIFS(RawData!$C$3:$C$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B22,RawData!$B$3:$B$6000,"&lt;"&amp;C22),0)</f>
@@ -3107,13 +3107,13 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="2"/>
-      <c r="B23" s="26" t="e">
+      <c r="B23" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
+        <v/>
       </c>
-      <c r="C23" s="26" t="e">
+      <c r="C23" s="23" t="str">
         <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+        <v/>
       </c>
       <c r="D23" s="27">
         <f>IF(COUNTIFS(RawData!$B$3:$B$6000,"&gt;="&amp;B23,RawData!$B$3:$B$6000,"&lt;"&amp;C23)&gt;0,AVERAGEIFS(RawData!$C$3:$C$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B23,RawData!$B$3:$B$6000,"&lt;"&amp;C23),0)</f>
@@ -3134,13 +3134,13 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="2"/>
-      <c r="B24" s="26" t="e">
+      <c r="B24" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
+        <v/>
       </c>
-      <c r="C24" s="26" t="e">
+      <c r="C24" s="23" t="str">
         <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+        <v/>
       </c>
       <c r="D24" s="27">
         <f>IF(COUNTIFS(RawData!$B$3:$B$6000,"&gt;="&amp;B24,RawData!$B$3:$B$6000,"&lt;"&amp;C24)&gt;0,AVERAGEIFS(RawData!$C$3:$C$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B24,RawData!$B$3:$B$6000,"&lt;"&amp;C24),0)</f>
@@ -3161,13 +3161,13 @@
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="2"/>
-      <c r="B25" s="26" t="e">
+      <c r="B25" s="26" t="str">
         <f t="shared" ref="B25:B30" si="4">C24</f>
-        <v>#VALUE!</v>
+        <v/>
       </c>
-      <c r="C25" s="26" t="e">
-        <f t="shared" ref="C25:C30" si="5">B25+(1/24)</f>
-        <v>#VALUE!</v>
+      <c r="C25" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
       <c r="D25" s="27">
         <f>IF(COUNTIFS(RawData!$B$3:$B$6000,"&gt;="&amp;B25,RawData!$B$3:$B$6000,"&lt;"&amp;C25)&gt;0,AVERAGEIFS(RawData!$C$3:$C$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B25,RawData!$B$3:$B$6000,"&lt;"&amp;C25),0)</f>
@@ -3188,13 +3188,13 @@
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="2"/>
-      <c r="B26" s="26" t="e">
+      <c r="B26" s="26" t="str">
         <f t="shared" si="4"/>
-        <v>#VALUE!</v>
+        <v/>
       </c>
-      <c r="C26" s="26" t="e">
-        <f t="shared" si="5"/>
-        <v>#VALUE!</v>
+      <c r="C26" s="23" t="str">
+        <f t="shared" ref="C26:C36" si="5">IF(B26&lt;&gt;"",B26+(1/24),"")</f>
+        <v/>
       </c>
       <c r="D26" s="27">
         <f>IF(COUNTIFS(RawData!$B$3:$B$6000,"&gt;="&amp;B26,RawData!$B$3:$B$6000,"&lt;"&amp;C26)&gt;0,AVERAGEIFS(RawData!$C$3:$C$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B26,RawData!$B$3:$B$6000,"&lt;"&amp;C26),0)</f>
@@ -3215,13 +3215,13 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="2"/>
-      <c r="B27" s="26" t="e">
+      <c r="B27" s="26" t="str">
         <f t="shared" si="4"/>
-        <v>#VALUE!</v>
+        <v/>
       </c>
-      <c r="C27" s="26" t="e">
+      <c r="C27" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>#VALUE!</v>
+        <v/>
       </c>
       <c r="D27" s="27">
         <f>IF(COUNTIFS(RawData!$B$3:$B$6000,"&gt;="&amp;B27,RawData!$B$3:$B$6000,"&lt;"&amp;C27)&gt;0,AVERAGEIFS(RawData!$C$3:$C$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B27,RawData!$B$3:$B$6000,"&lt;"&amp;C27),0)</f>
@@ -3242,13 +3242,13 @@
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="2"/>
-      <c r="B28" s="26" t="e">
+      <c r="B28" s="26" t="str">
         <f t="shared" si="4"/>
-        <v>#VALUE!</v>
+        <v/>
       </c>
-      <c r="C28" s="26" t="e">
+      <c r="C28" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>#VALUE!</v>
+        <v/>
       </c>
       <c r="D28" s="27">
         <f>IF(COUNTIFS(RawData!$B$3:$B$6000,"&gt;="&amp;B28,RawData!$B$3:$B$6000,"&lt;"&amp;C28)&gt;0,AVERAGEIFS(RawData!$C$3:$C$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B28,RawData!$B$3:$B$6000,"&lt;"&amp;C28),0)</f>
@@ -3269,13 +3269,13 @@
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="2"/>
-      <c r="B29" s="26" t="e">
+      <c r="B29" s="26" t="str">
         <f t="shared" si="4"/>
-        <v>#VALUE!</v>
+        <v/>
       </c>
-      <c r="C29" s="26" t="e">
+      <c r="C29" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>#VALUE!</v>
+        <v/>
       </c>
       <c r="D29" s="27">
         <f>IF(COUNTIFS(RawData!$B$3:$B$6000,"&gt;="&amp;B29,RawData!$B$3:$B$6000,"&lt;"&amp;C29)&gt;0,AVERAGEIFS(RawData!$C$3:$C$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B29,RawData!$B$3:$B$6000,"&lt;"&amp;C29),0)</f>
@@ -3296,13 +3296,13 @@
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="2"/>
-      <c r="B30" s="26" t="e">
+      <c r="B30" s="26" t="str">
         <f t="shared" si="4"/>
-        <v>#VALUE!</v>
+        <v/>
       </c>
-      <c r="C30" s="26" t="e">
+      <c r="C30" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>#VALUE!</v>
+        <v/>
       </c>
       <c r="D30" s="27">
         <f>IF(COUNTIFS(RawData!$B$3:$B$6000,"&gt;="&amp;B30,RawData!$B$3:$B$6000,"&lt;"&amp;C30)&gt;0,AVERAGEIFS(RawData!$C$3:$C$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B30,RawData!$B$3:$B$6000,"&lt;"&amp;C30),0)</f>
@@ -3323,13 +3323,13 @@
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="2"/>
-      <c r="B31" s="26" t="e">
+      <c r="B31" s="26" t="str">
         <f t="shared" ref="B31:B37" si="6">C30</f>
-        <v>#VALUE!</v>
+        <v/>
       </c>
-      <c r="C31" s="26" t="e">
-        <f t="shared" ref="C31:C37" si="7">B31+(1/24)</f>
-        <v>#VALUE!</v>
+      <c r="C31" s="23" t="str">
+        <f t="shared" si="5"/>
+        <v/>
       </c>
       <c r="D31" s="27">
         <f>IF(COUNTIFS(RawData!$B$3:$B$6000,"&gt;="&amp;B31,RawData!$B$3:$B$6000,"&lt;"&amp;C31)&gt;0,AVERAGEIFS(RawData!$C$3:$C$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B31,RawData!$B$3:$B$6000,"&lt;"&amp;C31),0)</f>
@@ -3350,13 +3350,13 @@
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="2"/>
-      <c r="B32" s="26" t="e">
+      <c r="B32" s="26" t="str">
         <f t="shared" si="6"/>
-        <v>#VALUE!</v>
+        <v/>
       </c>
-      <c r="C32" s="26" t="e">
-        <f t="shared" si="7"/>
-        <v>#VALUE!</v>
+      <c r="C32" s="23" t="str">
+        <f t="shared" si="5"/>
+        <v/>
       </c>
       <c r="D32" s="27">
         <f>IF(COUNTIFS(RawData!$B$3:$B$6000,"&gt;="&amp;B32,RawData!$B$3:$B$6000,"&lt;"&amp;C32)&gt;0,AVERAGEIFS(RawData!$C$3:$C$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B32,RawData!$B$3:$B$6000,"&lt;"&amp;C32),0)</f>
@@ -3377,13 +3377,13 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="2"/>
-      <c r="B33" s="26" t="e">
+      <c r="B33" s="26" t="str">
         <f t="shared" si="6"/>
-        <v>#VALUE!</v>
+        <v/>
       </c>
-      <c r="C33" s="26" t="e">
-        <f t="shared" si="7"/>
-        <v>#VALUE!</v>
+      <c r="C33" s="23" t="str">
+        <f t="shared" si="5"/>
+        <v/>
       </c>
       <c r="D33" s="27">
         <f>IF(COUNTIFS(RawData!$B$3:$B$6000,"&gt;="&amp;B33,RawData!$B$3:$B$6000,"&lt;"&amp;C33)&gt;0,AVERAGEIFS(RawData!$C$3:$C$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B33,RawData!$B$3:$B$6000,"&lt;"&amp;C33),0)</f>
@@ -3404,13 +3404,13 @@
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="2"/>
-      <c r="B34" s="26" t="e">
+      <c r="B34" s="26" t="str">
         <f t="shared" si="6"/>
-        <v>#VALUE!</v>
+        <v/>
       </c>
-      <c r="C34" s="26" t="e">
-        <f t="shared" si="7"/>
-        <v>#VALUE!</v>
+      <c r="C34" s="23" t="str">
+        <f t="shared" si="5"/>
+        <v/>
       </c>
       <c r="D34" s="27">
         <f>IF(COUNTIFS(RawData!$B$3:$B$6000,"&gt;="&amp;B34,RawData!$B$3:$B$6000,"&lt;"&amp;C34)&gt;0,AVERAGEIFS(RawData!$C$3:$C$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B34,RawData!$B$3:$B$6000,"&lt;"&amp;C34),0)</f>
@@ -3431,13 +3431,13 @@
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="2"/>
-      <c r="B35" s="26" t="e">
+      <c r="B35" s="26" t="str">
         <f t="shared" si="6"/>
-        <v>#VALUE!</v>
+        <v/>
       </c>
-      <c r="C35" s="26" t="e">
-        <f t="shared" si="7"/>
-        <v>#VALUE!</v>
+      <c r="C35" s="23" t="str">
+        <f t="shared" si="5"/>
+        <v/>
       </c>
       <c r="D35" s="27">
         <f>IF(COUNTIFS(RawData!$B$3:$B$6000,"&gt;="&amp;B35,RawData!$B$3:$B$6000,"&lt;"&amp;C35)&gt;0,AVERAGEIFS(RawData!$C$3:$C$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B35,RawData!$B$3:$B$6000,"&lt;"&amp;C35),0)</f>
@@ -3458,13 +3458,13 @@
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="2"/>
-      <c r="B36" s="26" t="e">
+      <c r="B36" s="26" t="str">
         <f t="shared" si="6"/>
-        <v>#VALUE!</v>
+        <v/>
       </c>
-      <c r="C36" s="26" t="e">
-        <f t="shared" si="7"/>
-        <v>#VALUE!</v>
+      <c r="C36" s="23" t="str">
+        <f t="shared" si="5"/>
+        <v/>
       </c>
       <c r="D36" s="27">
         <f>IF(COUNTIFS(RawData!$B$3:$B$6000,"&gt;="&amp;B36,RawData!$B$3:$B$6000,"&lt;"&amp;C36)&gt;0,AVERAGEIFS(RawData!$C$3:$C$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B36,RawData!$B$3:$B$6000,"&lt;"&amp;C36),0)</f>

</xml_diff>

<commit_message>
check report flow meter
</commit_message>
<xml_diff>
--- a/Report/flow.xlsx
+++ b/Report/flow.xlsx
@@ -1289,1055 +1289,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="zh-CN"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr defTabSz="914400">
-              <a:defRPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:t>Flow Rate</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.445941610522939"/>
-          <c:y val="0.0350262697022767"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="28575" cmpd="sng">
-          <a:noFill/>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="stacked"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Report!$A$13</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v/>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dLbls>
-            <c:delete val="1"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Report!$B$13:$B$36</c:f>
-              <c:strCache>
-                <c:ptCount val="24"/>
-                <c:pt idx="0" c:formatCode="hh:mm;@">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="1" c:formatCode="hh:mm;@">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="2" c:formatCode="hh:mm;@">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="3" c:formatCode="hh:mm;@">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="4" c:formatCode="hh:mm;@">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="5" c:formatCode="hh:mm;@">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="6" c:formatCode="hh:mm;@">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="7" c:formatCode="hh:mm;@">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="8" c:formatCode="hh:mm;@">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="9" c:formatCode="hh:mm;@">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="10" c:formatCode="hh:mm;@">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="11" c:formatCode="hh:mm;@">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="12" c:formatCode="hh:mm;@">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="13" c:formatCode="hh:mm;@">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="14" c:formatCode="hh:mm;@">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="15" c:formatCode="hh:mm;@">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="16" c:formatCode="hh:mm;@">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="17" c:formatCode="hh:mm;@">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="18" c:formatCode="hh:mm;@">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="19" c:formatCode="hh:mm;@">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="20" c:formatCode="hh:mm;@">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="21" c:formatCode="hh:mm;@">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="22" c:formatCode="hh:mm;@">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="23" c:formatCode="hh:mm;@">
-                  <c:v/>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Report!$D$13:$D$36</c:f>
-              <c:numCache>
-                <c:formatCode>0.00_ </c:formatCode>
-                <c:ptCount val="24"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="0"/>
-        <c:smooth val="0"/>
-        <c:axId val="976450309"/>
-        <c:axId val="542807230"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="976450309"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr defTabSz="914400">
-                  <a:defRPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:t>Waktu</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout>
-            <c:manualLayout>
-              <c:xMode val="edge"/>
-              <c:yMode val="edge"/>
-              <c:x val="0.479392578333868"/>
-              <c:y val="0.867900925694271"/>
-            </c:manualLayout>
-          </c:layout>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:title>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="542807230"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="542807230"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr defTabSz="914400">
-                  <a:defRPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:t>(L/min)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="0.00_ " sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="976450309"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="zero"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr lang="en-US"/>
-      </a:pPr>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
@@ -2361,7 +1312,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId2"/>
+        <a:blip r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2376,36 +1327,6 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>26035</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>182245</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame>
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="38100" y="7089775"/>
-        <a:ext cx="5937885" cy="2538095"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2671,8 +1592,8 @@
   <sheetPr/>
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="6"/>
@@ -3536,7 +2457,7 @@
   <dimension ref="B2:F6047"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="5"/>

</xml_diff>

<commit_message>
Flow meter report baru update
</commit_message>
<xml_diff>
--- a/Report/flow.xlsx
+++ b/Report/flow.xlsx
@@ -15,7 +15,31 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+  <si>
+    <t>PT. KANSAI PRAKARSA COATINGS</t>
+  </si>
+  <si>
+    <t>ENGINEERING UNIT CAT</t>
+  </si>
+  <si>
+    <t>LAPORAN PENGGUNAAN AIR</t>
+  </si>
+  <si>
+    <t>ALAT UKUR</t>
+  </si>
+  <si>
+    <t>FLOW METER ELECTROMAGNETIC</t>
+  </si>
+  <si>
+    <t>SUMBER</t>
+  </si>
+  <si>
+    <t>SUMUR TANAH 02</t>
+  </si>
+  <si>
+    <t>DATE UPDATE</t>
+  </si>
   <si>
     <t>Tanggal</t>
   </si>
@@ -29,10 +53,10 @@
     <t>Pemakaian Air</t>
   </si>
   <si>
-    <t>start</t>
+    <t>Start</t>
   </si>
   <si>
-    <t>finish</t>
+    <t>Finish</t>
   </si>
   <si>
     <t>M3/H</t>
@@ -45,6 +69,9 @@
   </si>
   <si>
     <t>L</t>
+  </si>
+  <si>
+    <t>AVERAGE | FLOW</t>
   </si>
   <si>
     <t>Time</t>
@@ -70,7 +97,7 @@
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -81,6 +108,20 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -230,12 +271,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -424,7 +471,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -459,6 +506,43 @@
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -580,137 +664,137 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -733,8 +817,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1011,6 +1125,49 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>51435</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>543560</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 4" descr="logo"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="51435" y="171450"/>
+          <a:ext cx="1101725" cy="339725"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
@@ -1269,690 +1426,788 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A11:G36"/>
+  <dimension ref="A2:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="6"/>
   <cols>
-    <col min="3" max="3" width="12.8181818181818"/>
+    <col min="2" max="2" width="10.2727272727273" customWidth="1"/>
+    <col min="3" max="3" width="10.3636363636364" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="11" spans="1:7">
-      <c r="A11" s="10" t="s">
+    <row r="2" spans="3:3">
+      <c r="C2" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="10" t="s">
+    </row>
+    <row r="3" spans="3:3">
+      <c r="C3" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="10"/>
-      <c r="D11" t="s">
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="12"/>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
         <v>3</v>
       </c>
-      <c r="G11" s="10"/>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="10"/>
-      <c r="B12" t="s">
+      <c r="B7" t="s">
         <v>4</v>
       </c>
-      <c r="C12" t="s">
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
         <v>5</v>
       </c>
-      <c r="D12" t="s">
+      <c r="B8" t="s">
         <v>6</v>
       </c>
-      <c r="E12" t="s">
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="F12" t="s">
-        <v>8</v>
-      </c>
-      <c r="G12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" t="str">
+      <c r="B9" t="str">
         <f>RawData!F3</f>
         <v/>
       </c>
-      <c r="B13" t="str">
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="13"/>
+      <c r="D11" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="12"/>
+      <c r="F11" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" s="13"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="13"/>
+      <c r="B12" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="16" t="str">
+        <f>RawData!F3</f>
+        <v/>
+      </c>
+      <c r="B13" s="16" t="str">
         <f>A13</f>
         <v/>
       </c>
-      <c r="C13" t="e">
+      <c r="C13" s="16" t="e">
         <f>B13+(1/24)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="16">
         <f>IF(COUNTIFS(RawData!$B$3:$B$6000,"&gt;="&amp;B13,RawData!$B$3:$B$6000,"&lt;"&amp;C13)&gt;0,AVERAGEIFS(RawData!$C$3:$C$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B13,RawData!$B$3:$B$6000,"&lt;"&amp;C13),0)</f>
         <v>0</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="16">
         <f>D13*16.667</f>
         <v>0</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="16">
         <f>_xlfn.MAXIFS(RawData!$D$3:$D$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B13,RawData!$B$3:$B$6000,"&lt;"&amp;C13)-_xlfn.MINIFS(RawData!$D$3:$D$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B13,RawData!$B$3:$B$6000,"&lt;"&amp;C13)</f>
         <v>0</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="16">
         <f>F13*1000</f>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:7">
-      <c r="B14" t="e">
+    <row r="14" spans="1:7">
+      <c r="A14" s="16"/>
+      <c r="B14" s="16" t="e">
         <f>C13</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C14" t="e">
+      <c r="C14" s="16" t="e">
         <f t="shared" ref="C14:C30" si="0">B14+(1/24)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="16">
         <f>IF(COUNTIFS(RawData!$B$3:$B$6000,"&gt;="&amp;B14,RawData!$B$3:$B$6000,"&lt;"&amp;C14)&gt;0,AVERAGEIFS(RawData!$C$3:$C$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B14,RawData!$B$3:$B$6000,"&lt;"&amp;C14),0)</f>
         <v>0</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="16">
         <f t="shared" ref="E14:E36" si="1">D14*16.667</f>
         <v>0</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="16">
         <f>_xlfn.MAXIFS(RawData!$D$3:$D$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B14,RawData!$B$3:$B$6000,"&lt;"&amp;C14)-_xlfn.MINIFS(RawData!$D$3:$D$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B14,RawData!$B$3:$B$6000,"&lt;"&amp;C14)</f>
         <v>0</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="16">
         <f t="shared" ref="G14:G36" si="2">F14*1000</f>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:7">
-      <c r="B15" t="e">
+    <row r="15" spans="1:7">
+      <c r="A15" s="16"/>
+      <c r="B15" s="16" t="e">
         <f t="shared" ref="B15:B30" si="3">C14</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C15" t="e">
+      <c r="C15" s="16" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="16">
         <f>IF(COUNTIFS(RawData!$B$3:$B$6000,"&gt;="&amp;B15,RawData!$B$3:$B$6000,"&lt;"&amp;C15)&gt;0,AVERAGEIFS(RawData!$C$3:$C$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B15,RawData!$B$3:$B$6000,"&lt;"&amp;C15),0)</f>
         <v>0</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="16">
         <f>_xlfn.MAXIFS(RawData!$D$3:$D$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B15,RawData!$B$3:$B$6000,"&lt;"&amp;C15)-_xlfn.MINIFS(RawData!$D$3:$D$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B15,RawData!$B$3:$B$6000,"&lt;"&amp;C15)</f>
         <v>0</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:7">
-      <c r="B16" t="e">
+    <row r="16" spans="1:7">
+      <c r="A16" s="16"/>
+      <c r="B16" s="16" t="e">
         <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
-      <c r="C16" t="e">
+      <c r="C16" s="16" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="16">
         <f>IF(COUNTIFS(RawData!$B$3:$B$6000,"&gt;="&amp;B16,RawData!$B$3:$B$6000,"&lt;"&amp;C16)&gt;0,AVERAGEIFS(RawData!$C$3:$C$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B16,RawData!$B$3:$B$6000,"&lt;"&amp;C16),0)</f>
         <v>0</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="16">
         <f>_xlfn.MAXIFS(RawData!$D$3:$D$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B16,RawData!$B$3:$B$6000,"&lt;"&amp;C16)-_xlfn.MINIFS(RawData!$D$3:$D$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B16,RawData!$B$3:$B$6000,"&lt;"&amp;C16)</f>
         <v>0</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:7">
-      <c r="B17" t="e">
+    <row r="17" spans="1:7">
+      <c r="A17" s="16"/>
+      <c r="B17" s="16" t="e">
         <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
-      <c r="C17" t="e">
+      <c r="C17" s="16" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="16">
         <f>IF(COUNTIFS(RawData!$B$3:$B$6000,"&gt;="&amp;B17,RawData!$B$3:$B$6000,"&lt;"&amp;C17)&gt;0,AVERAGEIFS(RawData!$C$3:$C$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B17,RawData!$B$3:$B$6000,"&lt;"&amp;C17),0)</f>
         <v>0</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="16">
         <f>_xlfn.MAXIFS(RawData!$D$3:$D$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B17,RawData!$B$3:$B$6000,"&lt;"&amp;C17)-_xlfn.MINIFS(RawData!$D$3:$D$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B17,RawData!$B$3:$B$6000,"&lt;"&amp;C17)</f>
         <v>0</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:7">
-      <c r="B18" t="e">
+    <row r="18" spans="1:7">
+      <c r="A18" s="16"/>
+      <c r="B18" s="16" t="e">
         <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
-      <c r="C18" t="e">
+      <c r="C18" s="16" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="16">
         <f>IF(COUNTIFS(RawData!$B$3:$B$6000,"&gt;="&amp;B18,RawData!$B$3:$B$6000,"&lt;"&amp;C18)&gt;0,AVERAGEIFS(RawData!$C$3:$C$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B18,RawData!$B$3:$B$6000,"&lt;"&amp;C18),0)</f>
         <v>0</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="16">
         <f>_xlfn.MAXIFS(RawData!$D$3:$D$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B18,RawData!$B$3:$B$6000,"&lt;"&amp;C18)-_xlfn.MINIFS(RawData!$D$3:$D$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B18,RawData!$B$3:$B$6000,"&lt;"&amp;C18)</f>
         <v>0</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:7">
-      <c r="B19" t="e">
+    <row r="19" spans="1:7">
+      <c r="A19" s="16"/>
+      <c r="B19" s="16" t="e">
         <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
-      <c r="C19" t="e">
+      <c r="C19" s="16" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="16">
         <f>IF(COUNTIFS(RawData!$B$3:$B$6000,"&gt;="&amp;B19,RawData!$B$3:$B$6000,"&lt;"&amp;C19)&gt;0,AVERAGEIFS(RawData!$C$3:$C$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B19,RawData!$B$3:$B$6000,"&lt;"&amp;C19),0)</f>
         <v>0</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="16">
         <f>_xlfn.MAXIFS(RawData!$D$3:$D$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B19,RawData!$B$3:$B$6000,"&lt;"&amp;C19)-_xlfn.MINIFS(RawData!$D$3:$D$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B19,RawData!$B$3:$B$6000,"&lt;"&amp;C19)</f>
         <v>0</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:7">
-      <c r="B20" t="e">
+    <row r="20" spans="1:7">
+      <c r="A20" s="16"/>
+      <c r="B20" s="16" t="e">
         <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
-      <c r="C20" t="e">
+      <c r="C20" s="16" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="16">
         <f>IF(COUNTIFS(RawData!$B$3:$B$6000,"&gt;="&amp;B20,RawData!$B$3:$B$6000,"&lt;"&amp;C20)&gt;0,AVERAGEIFS(RawData!$C$3:$C$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B20,RawData!$B$3:$B$6000,"&lt;"&amp;C20),0)</f>
         <v>0</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="16">
         <f>_xlfn.MAXIFS(RawData!$D$3:$D$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B20,RawData!$B$3:$B$6000,"&lt;"&amp;C20)-_xlfn.MINIFS(RawData!$D$3:$D$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B20,RawData!$B$3:$B$6000,"&lt;"&amp;C20)</f>
         <v>0</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:7">
-      <c r="B21" t="e">
+    <row r="21" spans="1:7">
+      <c r="A21" s="16"/>
+      <c r="B21" s="16" t="e">
         <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
-      <c r="C21" t="e">
+      <c r="C21" s="16" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="16">
         <f>IF(COUNTIFS(RawData!$B$3:$B$6000,"&gt;="&amp;B21,RawData!$B$3:$B$6000,"&lt;"&amp;C21)&gt;0,AVERAGEIFS(RawData!$C$3:$C$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B21,RawData!$B$3:$B$6000,"&lt;"&amp;C21),0)</f>
         <v>0</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="16">
         <f>_xlfn.MAXIFS(RawData!$D$3:$D$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B21,RawData!$B$3:$B$6000,"&lt;"&amp;C21)-_xlfn.MINIFS(RawData!$D$3:$D$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B21,RawData!$B$3:$B$6000,"&lt;"&amp;C21)</f>
         <v>0</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:7">
-      <c r="B22" t="e">
+    <row r="22" spans="1:7">
+      <c r="A22" s="16"/>
+      <c r="B22" s="16" t="e">
         <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
-      <c r="C22" t="e">
+      <c r="C22" s="16" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="16">
         <f>IF(COUNTIFS(RawData!$B$3:$B$6000,"&gt;="&amp;B22,RawData!$B$3:$B$6000,"&lt;"&amp;C22)&gt;0,AVERAGEIFS(RawData!$C$3:$C$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B22,RawData!$B$3:$B$6000,"&lt;"&amp;C22),0)</f>
         <v>0</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="16">
         <f>_xlfn.MAXIFS(RawData!$D$3:$D$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B22,RawData!$B$3:$B$6000,"&lt;"&amp;C22)-_xlfn.MINIFS(RawData!$D$3:$D$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B22,RawData!$B$3:$B$6000,"&lt;"&amp;C22)</f>
         <v>0</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:7">
-      <c r="B23" t="e">
+    <row r="23" spans="1:7">
+      <c r="A23" s="16"/>
+      <c r="B23" s="16" t="e">
         <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
-      <c r="C23" t="e">
+      <c r="C23" s="16" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="16">
         <f>IF(COUNTIFS(RawData!$B$3:$B$6000,"&gt;="&amp;B23,RawData!$B$3:$B$6000,"&lt;"&amp;C23)&gt;0,AVERAGEIFS(RawData!$C$3:$C$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B23,RawData!$B$3:$B$6000,"&lt;"&amp;C23),0)</f>
         <v>0</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="16">
         <f>_xlfn.MAXIFS(RawData!$D$3:$D$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B23,RawData!$B$3:$B$6000,"&lt;"&amp;C23)-_xlfn.MINIFS(RawData!$D$3:$D$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B23,RawData!$B$3:$B$6000,"&lt;"&amp;C23)</f>
         <v>0</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:7">
-      <c r="B24" t="e">
+    <row r="24" spans="1:7">
+      <c r="A24" s="16"/>
+      <c r="B24" s="16" t="e">
         <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
-      <c r="C24" t="e">
+      <c r="C24" s="16" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="16">
         <f>IF(COUNTIFS(RawData!$B$3:$B$6000,"&gt;="&amp;B24,RawData!$B$3:$B$6000,"&lt;"&amp;C24)&gt;0,AVERAGEIFS(RawData!$C$3:$C$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B24,RawData!$B$3:$B$6000,"&lt;"&amp;C24),0)</f>
         <v>0</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="16">
         <f>_xlfn.MAXIFS(RawData!$D$3:$D$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B24,RawData!$B$3:$B$6000,"&lt;"&amp;C24)-_xlfn.MINIFS(RawData!$D$3:$D$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B24,RawData!$B$3:$B$6000,"&lt;"&amp;C24)</f>
         <v>0</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:7">
-      <c r="B25" t="e">
+    <row r="25" spans="1:7">
+      <c r="A25" s="16"/>
+      <c r="B25" s="16" t="e">
         <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
-      <c r="C25" t="e">
+      <c r="C25" s="16" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="16">
         <f>IF(COUNTIFS(RawData!$B$3:$B$6000,"&gt;="&amp;B25,RawData!$B$3:$B$6000,"&lt;"&amp;C25)&gt;0,AVERAGEIFS(RawData!$C$3:$C$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B25,RawData!$B$3:$B$6000,"&lt;"&amp;C25),0)</f>
         <v>0</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="16">
         <f>_xlfn.MAXIFS(RawData!$D$3:$D$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B25,RawData!$B$3:$B$6000,"&lt;"&amp;C25)-_xlfn.MINIFS(RawData!$D$3:$D$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B25,RawData!$B$3:$B$6000,"&lt;"&amp;C25)</f>
         <v>0</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:7">
-      <c r="B26" t="e">
+    <row r="26" spans="1:7">
+      <c r="A26" s="16"/>
+      <c r="B26" s="16" t="e">
         <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
-      <c r="C26" t="e">
+      <c r="C26" s="16" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="16">
         <f>IF(COUNTIFS(RawData!$B$3:$B$6000,"&gt;="&amp;B26,RawData!$B$3:$B$6000,"&lt;"&amp;C26)&gt;0,AVERAGEIFS(RawData!$C$3:$C$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B26,RawData!$B$3:$B$6000,"&lt;"&amp;C26),0)</f>
         <v>0</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="16">
         <f>_xlfn.MAXIFS(RawData!$D$3:$D$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B26,RawData!$B$3:$B$6000,"&lt;"&amp;C26)-_xlfn.MINIFS(RawData!$D$3:$D$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B26,RawData!$B$3:$B$6000,"&lt;"&amp;C26)</f>
         <v>0</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:7">
-      <c r="B27" t="e">
+    <row r="27" spans="1:7">
+      <c r="A27" s="16"/>
+      <c r="B27" s="16" t="e">
         <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
-      <c r="C27" t="e">
+      <c r="C27" s="16" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="16">
         <f>IF(COUNTIFS(RawData!$B$3:$B$6000,"&gt;="&amp;B27,RawData!$B$3:$B$6000,"&lt;"&amp;C27)&gt;0,AVERAGEIFS(RawData!$C$3:$C$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B27,RawData!$B$3:$B$6000,"&lt;"&amp;C27),0)</f>
         <v>0</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="16">
         <f>_xlfn.MAXIFS(RawData!$D$3:$D$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B27,RawData!$B$3:$B$6000,"&lt;"&amp;C27)-_xlfn.MINIFS(RawData!$D$3:$D$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B27,RawData!$B$3:$B$6000,"&lt;"&amp;C27)</f>
         <v>0</v>
       </c>
-      <c r="G27">
+      <c r="G27" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:7">
-      <c r="B28" t="e">
+    <row r="28" spans="1:7">
+      <c r="A28" s="16"/>
+      <c r="B28" s="16" t="e">
         <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
-      <c r="C28" t="e">
+      <c r="C28" s="16" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="16">
         <f>IF(COUNTIFS(RawData!$B$3:$B$6000,"&gt;="&amp;B28,RawData!$B$3:$B$6000,"&lt;"&amp;C28)&gt;0,AVERAGEIFS(RawData!$C$3:$C$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B28,RawData!$B$3:$B$6000,"&lt;"&amp;C28),0)</f>
         <v>0</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="16">
         <f>_xlfn.MAXIFS(RawData!$D$3:$D$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B28,RawData!$B$3:$B$6000,"&lt;"&amp;C28)-_xlfn.MINIFS(RawData!$D$3:$D$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B28,RawData!$B$3:$B$6000,"&lt;"&amp;C28)</f>
         <v>0</v>
       </c>
-      <c r="G28">
+      <c r="G28" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:7">
-      <c r="B29" t="e">
+    <row r="29" spans="1:7">
+      <c r="A29" s="16"/>
+      <c r="B29" s="16" t="e">
         <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
-      <c r="C29" t="e">
+      <c r="C29" s="16" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="16">
         <f>IF(COUNTIFS(RawData!$B$3:$B$6000,"&gt;="&amp;B29,RawData!$B$3:$B$6000,"&lt;"&amp;C29)&gt;0,AVERAGEIFS(RawData!$C$3:$C$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B29,RawData!$B$3:$B$6000,"&lt;"&amp;C29),0)</f>
         <v>0</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F29">
+      <c r="F29" s="16">
         <f>_xlfn.MAXIFS(RawData!$D$3:$D$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B29,RawData!$B$3:$B$6000,"&lt;"&amp;C29)-_xlfn.MINIFS(RawData!$D$3:$D$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B29,RawData!$B$3:$B$6000,"&lt;"&amp;C29)</f>
         <v>0</v>
       </c>
-      <c r="G29">
+      <c r="G29" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:7">
-      <c r="B30" t="e">
+    <row r="30" spans="1:7">
+      <c r="A30" s="16"/>
+      <c r="B30" s="16" t="e">
         <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
-      <c r="C30" t="e">
+      <c r="C30" s="16" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="16">
         <f>IF(COUNTIFS(RawData!$B$3:$B$6000,"&gt;="&amp;B30,RawData!$B$3:$B$6000,"&lt;"&amp;C30)&gt;0,AVERAGEIFS(RawData!$C$3:$C$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B30,RawData!$B$3:$B$6000,"&lt;"&amp;C30),0)</f>
         <v>0</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F30">
+      <c r="F30" s="16">
         <f>_xlfn.MAXIFS(RawData!$D$3:$D$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B30,RawData!$B$3:$B$6000,"&lt;"&amp;C30)-_xlfn.MINIFS(RawData!$D$3:$D$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B30,RawData!$B$3:$B$6000,"&lt;"&amp;C30)</f>
         <v>0</v>
       </c>
-      <c r="G30">
+      <c r="G30" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:7">
-      <c r="B31" t="e">
+    <row r="31" spans="1:7">
+      <c r="A31" s="16"/>
+      <c r="B31" s="16" t="e">
         <f t="shared" ref="B31:B36" si="4">C30</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C31" t="e">
+      <c r="C31" s="16" t="e">
         <f t="shared" ref="C31:C36" si="5">B31+(1/24)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="16">
         <f>IF(COUNTIFS(RawData!$B$3:$B$6000,"&gt;="&amp;B31,RawData!$B$3:$B$6000,"&lt;"&amp;C31)&gt;0,AVERAGEIFS(RawData!$C$3:$C$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B31,RawData!$B$3:$B$6000,"&lt;"&amp;C31),0)</f>
         <v>0</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F31">
+      <c r="F31" s="16">
         <f>_xlfn.MAXIFS(RawData!$D$3:$D$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B31,RawData!$B$3:$B$6000,"&lt;"&amp;C31)-_xlfn.MINIFS(RawData!$D$3:$D$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B31,RawData!$B$3:$B$6000,"&lt;"&amp;C31)</f>
         <v>0</v>
       </c>
-      <c r="G31">
+      <c r="G31" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:7">
-      <c r="B32" t="e">
+    <row r="32" spans="1:7">
+      <c r="A32" s="16"/>
+      <c r="B32" s="16" t="e">
         <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
-      <c r="C32" t="e">
+      <c r="C32" s="16" t="e">
         <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="16">
         <f>IF(COUNTIFS(RawData!$B$3:$B$6000,"&gt;="&amp;B32,RawData!$B$3:$B$6000,"&lt;"&amp;C32)&gt;0,AVERAGEIFS(RawData!$C$3:$C$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B32,RawData!$B$3:$B$6000,"&lt;"&amp;C32),0)</f>
         <v>0</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F32">
+      <c r="F32" s="16">
         <f>_xlfn.MAXIFS(RawData!$D$3:$D$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B32,RawData!$B$3:$B$6000,"&lt;"&amp;C32)-_xlfn.MINIFS(RawData!$D$3:$D$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B32,RawData!$B$3:$B$6000,"&lt;"&amp;C32)</f>
         <v>0</v>
       </c>
-      <c r="G32">
+      <c r="G32" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:7">
-      <c r="B33" t="e">
+    <row r="33" spans="1:7">
+      <c r="A33" s="16"/>
+      <c r="B33" s="16" t="e">
         <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
-      <c r="C33" t="e">
+      <c r="C33" s="16" t="e">
         <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="16">
         <f>IF(COUNTIFS(RawData!$B$3:$B$6000,"&gt;="&amp;B33,RawData!$B$3:$B$6000,"&lt;"&amp;C33)&gt;0,AVERAGEIFS(RawData!$C$3:$C$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B33,RawData!$B$3:$B$6000,"&lt;"&amp;C33),0)</f>
         <v>0</v>
       </c>
-      <c r="E33">
+      <c r="E33" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F33">
+      <c r="F33" s="16">
         <f>_xlfn.MAXIFS(RawData!$D$3:$D$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B33,RawData!$B$3:$B$6000,"&lt;"&amp;C33)-_xlfn.MINIFS(RawData!$D$3:$D$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B33,RawData!$B$3:$B$6000,"&lt;"&amp;C33)</f>
         <v>0</v>
       </c>
-      <c r="G33">
+      <c r="G33" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:7">
-      <c r="B34" t="e">
+    <row r="34" spans="1:7">
+      <c r="A34" s="16"/>
+      <c r="B34" s="16" t="e">
         <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
-      <c r="C34" t="e">
+      <c r="C34" s="16" t="e">
         <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
-      <c r="D34">
+      <c r="D34" s="16">
         <f>IF(COUNTIFS(RawData!$B$3:$B$6000,"&gt;="&amp;B34,RawData!$B$3:$B$6000,"&lt;"&amp;C34)&gt;0,AVERAGEIFS(RawData!$C$3:$C$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B34,RawData!$B$3:$B$6000,"&lt;"&amp;C34),0)</f>
         <v>0</v>
       </c>
-      <c r="E34">
+      <c r="E34" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F34">
+      <c r="F34" s="16">
         <f>_xlfn.MAXIFS(RawData!$D$3:$D$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B34,RawData!$B$3:$B$6000,"&lt;"&amp;C34)-_xlfn.MINIFS(RawData!$D$3:$D$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B34,RawData!$B$3:$B$6000,"&lt;"&amp;C34)</f>
         <v>0</v>
       </c>
-      <c r="G34">
+      <c r="G34" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:7">
-      <c r="B35" t="e">
+    <row r="35" spans="1:7">
+      <c r="A35" s="16"/>
+      <c r="B35" s="16" t="e">
         <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
-      <c r="C35" t="e">
+      <c r="C35" s="16" t="e">
         <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
-      <c r="D35">
+      <c r="D35" s="16">
         <f>IF(COUNTIFS(RawData!$B$3:$B$6000,"&gt;="&amp;B35,RawData!$B$3:$B$6000,"&lt;"&amp;C35)&gt;0,AVERAGEIFS(RawData!$C$3:$C$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B35,RawData!$B$3:$B$6000,"&lt;"&amp;C35),0)</f>
         <v>0</v>
       </c>
-      <c r="E35">
+      <c r="E35" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F35">
+      <c r="F35" s="16">
         <f>_xlfn.MAXIFS(RawData!$D$3:$D$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B35,RawData!$B$3:$B$6000,"&lt;"&amp;C35)-_xlfn.MINIFS(RawData!$D$3:$D$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B35,RawData!$B$3:$B$6000,"&lt;"&amp;C35)</f>
         <v>0</v>
       </c>
-      <c r="G35">
+      <c r="G35" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:7">
-      <c r="B36" t="e">
+    <row r="36" spans="1:7">
+      <c r="A36" s="16"/>
+      <c r="B36" s="16" t="e">
         <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
-      <c r="C36" t="e">
+      <c r="C36" s="16" t="e">
         <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
-      <c r="D36">
+      <c r="D36" s="16">
         <f>IF(COUNTIFS(RawData!$B$3:$B$6000,"&gt;="&amp;B36,RawData!$B$3:$B$6000,"&lt;"&amp;C36)&gt;0,AVERAGEIFS(RawData!$C$3:$C$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B36,RawData!$B$3:$B$6000,"&lt;"&amp;C36),0)</f>
         <v>0</v>
       </c>
-      <c r="E36">
+      <c r="E36" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F36">
+      <c r="F36" s="16">
         <f>_xlfn.MAXIFS(RawData!$D$3:$D$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B36,RawData!$B$3:$B$6000,"&lt;"&amp;C36)-_xlfn.MINIFS(RawData!$D$3:$D$6000,RawData!$B$3:$B$6000,"&gt;="&amp;B36,RawData!$B$3:$B$6000,"&lt;"&amp;C36)</f>
         <v>0</v>
       </c>
-      <c r="G36">
+      <c r="G36" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
+    <row r="37" spans="1:7">
+      <c r="A37" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B37" s="18"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="19">
+        <f>AVERAGE(D13:D36)</f>
+        <v>0</v>
+      </c>
+      <c r="E37" s="19">
+        <f>AVERAGE(E13:E36)</f>
+        <v>0</v>
+      </c>
+      <c r="F37" s="20">
+        <f>SUM(F13:F36)</f>
+        <v>0</v>
+      </c>
+      <c r="G37" s="20">
+        <f>SUM(G13:G36)</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="6">
+    <mergeCell ref="A5:G5"/>
     <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:E11"/>
     <mergeCell ref="F11:G11"/>
+    <mergeCell ref="A37:C37"/>
     <mergeCell ref="A11:A12"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1976,24 +2231,22 @@
   <sheetData>
     <row r="2" s="1" customFormat="1" spans="2:6">
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
-      <c r="E2" s="1"/>
       <c r="F2" s="3" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="1" spans="2:6">
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
-      <c r="E3" s="1"/>
       <c r="F3" s="6" t="str">
         <f>IF(ISNUMBER(MROUND(LARGE(B3:B6000,1),1)),MROUND(LARGE(B3:B6000,1),1),"")</f>
         <v/>
@@ -2003,7 +2256,6 @@
       <c r="B4" s="4"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
-      <c r="E4" s="1"/>
       <c r="F4" s="6" t="str">
         <f>IF(ISNUMBER(F3),IF((F3)&gt;SMALL($B$3:$B$6000,1),(F3-1),""),"")</f>
         <v/>
@@ -2013,7 +2265,6 @@
       <c r="B5" s="4"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
-      <c r="E5" s="1"/>
       <c r="F5" s="6" t="str">
         <f>IF(ISNUMBER(F4),IF((F4)&gt;SMALL($B$3:$B$6000,1),(F4-1),""),"")</f>
         <v/>
@@ -2023,7 +2274,6 @@
       <c r="B6" s="4"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
-      <c r="E6" s="1"/>
       <c r="F6" s="6" t="str">
         <f>IF(ISNUMBER(F5),IF((F5)&gt;SMALL($B$3:$B$6000,1),(F5-1),""),"")</f>
         <v/>
@@ -2033,7 +2283,6 @@
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
-      <c r="E7" s="1"/>
       <c r="F7" s="6" t="str">
         <f>IF(ISNUMBER(F6),IF((F6)&gt;SMALL($B$3:$B$6000,1),(F6-1),""),"")</f>
         <v/>
@@ -2043,7 +2292,6 @@
       <c r="B8" s="4"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
-      <c r="E8" s="1"/>
       <c r="F8" s="6" t="str">
         <f>IF(ISNUMBER(F7),IF((F7)&gt;SMALL($B$3:$B$6000,1),(F7-1),""),"")</f>
         <v/>
@@ -2053,7 +2301,6 @@
       <c r="B9" s="4"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
-      <c r="E9" s="1"/>
       <c r="F9" s="6" t="str">
         <f>IF(ISNUMBER(F8),IF((F8)&gt;SMALL($B$3:$B$6000,1),(F8-1),""),"")</f>
         <v/>
@@ -2063,7 +2310,6 @@
       <c r="B10" s="4"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
-      <c r="E10" s="1"/>
       <c r="F10" s="6" t="str">
         <f>IF(ISNUMBER(F9),IF((F9)&gt;SMALL($B$3:$B$6000,1),(F9-1),""),"")</f>
         <v/>
@@ -2073,7 +2319,6 @@
       <c r="B11" s="4"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
-      <c r="E11" s="1"/>
       <c r="F11" s="6" t="str">
         <f>IF(ISNUMBER(F10),IF((F10)&gt;SMALL($B$3:$B$6000,1),(F10-1),""),"")</f>
         <v/>
@@ -2083,7 +2328,6 @@
       <c r="B12" s="4"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
-      <c r="E12" s="1"/>
       <c r="F12" s="6" t="str">
         <f>IF(ISNUMBER(F11),IF((F11)&gt;SMALL($B$3:$B$6000,1),(F11-1),""),"")</f>
         <v/>
@@ -2093,7 +2337,6 @@
       <c r="B13" s="4"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
-      <c r="E13" s="1"/>
       <c r="F13" s="6" t="str">
         <f>IF(ISNUMBER(F12),IF((F12)&gt;SMALL($B$3:$B$6000,1),(F12-1),""),"")</f>
         <v/>
@@ -2103,7 +2346,6 @@
       <c r="B14" s="4"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
-      <c r="E14" s="1"/>
       <c r="F14" s="6" t="str">
         <f>IF(ISNUMBER(F13),IF((F13)&gt;SMALL($B$3:$B$6000,1),(F13-1),""),"")</f>
         <v/>
@@ -2113,7 +2355,6 @@
       <c r="B15" s="4"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
-      <c r="E15" s="1"/>
       <c r="F15" s="6" t="str">
         <f>IF(ISNUMBER(F14),IF((F14)&gt;SMALL($B$3:$B$6000,1),(F14-1),""),"")</f>
         <v/>
@@ -2123,7 +2364,6 @@
       <c r="B16" s="4"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
-      <c r="E16" s="1"/>
       <c r="F16" s="6" t="str">
         <f>IF(ISNUMBER(F15),IF((F15)&gt;SMALL($B$3:$B$6000,1),(F15-1),""),"")</f>
         <v/>
@@ -2133,7 +2373,6 @@
       <c r="B17" s="4"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
-      <c r="E17" s="1"/>
       <c r="F17" s="6" t="str">
         <f>IF(ISNUMBER(F16),IF((F16)&gt;SMALL($B$3:$B$6000,1),(F16-1),""),"")</f>
         <v/>
@@ -2143,7 +2382,6 @@
       <c r="B18" s="4"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
-      <c r="E18" s="1"/>
       <c r="F18" s="6" t="str">
         <f>IF(ISNUMBER(F17),IF((F17)&gt;SMALL($B$3:$B$6000,1),(F17-1),""),"")</f>
         <v/>
@@ -2153,7 +2391,6 @@
       <c r="B19" s="4"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
-      <c r="E19" s="1"/>
       <c r="F19" s="6" t="str">
         <f>IF(ISNUMBER(F18),IF((F18)&gt;SMALL($B$3:$B$6000,1),(F18-1),""),"")</f>
         <v/>
@@ -2163,7 +2400,6 @@
       <c r="B20" s="4"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
-      <c r="E20" s="1"/>
       <c r="F20" s="6" t="str">
         <f>IF(ISNUMBER(F19),IF((F19)&gt;SMALL($B$3:$B$6000,1),(F19-1),""),"")</f>
         <v/>
@@ -2173,7 +2409,6 @@
       <c r="B21" s="4"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
-      <c r="E21" s="1"/>
       <c r="F21" s="6" t="str">
         <f>IF(ISNUMBER(F20),IF((F20)&gt;SMALL($B$3:$B$6000,1),(F20-1),""),"")</f>
         <v/>
@@ -2183,7 +2418,6 @@
       <c r="B22" s="4"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
-      <c r="E22" s="1"/>
       <c r="F22" s="6" t="str">
         <f>IF(ISNUMBER(F21),IF((F21)&gt;SMALL($B$3:$B$6000,1),(F21-1),""),"")</f>
         <v/>
@@ -2193,7 +2427,6 @@
       <c r="B23" s="4"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
-      <c r="E23" s="1"/>
       <c r="F23" s="6" t="str">
         <f>IF(ISNUMBER(F22),IF((F22)&gt;SMALL($B$3:$B$6000,1),(F22-1),""),"")</f>
         <v/>
@@ -2203,7 +2436,6 @@
       <c r="B24" s="4"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
-      <c r="E24" s="1"/>
       <c r="F24" s="6" t="str">
         <f>IF(ISNUMBER(F23),IF((F23)&gt;SMALL($B$3:$B$6000,1),(F23-1),""),"")</f>
         <v/>
@@ -2213,7 +2445,6 @@
       <c r="B25" s="4"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
-      <c r="E25" s="1"/>
       <c r="F25" s="6" t="str">
         <f>IF(ISNUMBER(F24),IF((F24)&gt;SMALL($B$3:$B$6000,1),(F24-1),""),"")</f>
         <v/>
@@ -2223,7 +2454,6 @@
       <c r="B26" s="4"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
-      <c r="E26" s="1"/>
       <c r="F26" s="6" t="str">
         <f>IF(ISNUMBER(F25),IF((F25)&gt;SMALL($B$3:$B$6000,1),(F25-1),""),"")</f>
         <v/>
@@ -2233,7 +2463,6 @@
       <c r="B27" s="4"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
-      <c r="E27" s="1"/>
       <c r="F27" s="6" t="str">
         <f>IF(ISNUMBER(F26),IF((F26)&gt;SMALL($B$3:$B$6000,1),(F26-1),""),"")</f>
         <v/>
@@ -2243,7 +2472,6 @@
       <c r="B28" s="4"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
-      <c r="E28" s="1"/>
       <c r="F28" s="6" t="str">
         <f>IF(ISNUMBER(F27),IF((F27)&gt;SMALL($B$3:$B$6000,1),(F27-1),""),"")</f>
         <v/>
@@ -2253,7 +2481,6 @@
       <c r="B29" s="4"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
-      <c r="E29" s="1"/>
       <c r="F29" s="6" t="str">
         <f>IF(ISNUMBER(F28),IF((F28)&gt;SMALL($B$3:$B$6000,1),(F28-1),""),"")</f>
         <v/>
@@ -2263,7 +2490,6 @@
       <c r="B30" s="4"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
-      <c r="E30" s="1"/>
       <c r="F30" s="6" t="str">
         <f>IF(ISNUMBER(F29),IF((F29)&gt;SMALL($B$3:$B$6000,1),(F29-1),""),"")</f>
         <v/>
@@ -2273,7 +2499,6 @@
       <c r="B31" s="4"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
-      <c r="E31" s="1"/>
       <c r="F31" s="6" t="str">
         <f>IF(ISNUMBER(F30),IF((F30)&gt;SMALL($B$3:$B$6000,1),(F30-1),""),"")</f>
         <v/>
@@ -2283,7 +2508,6 @@
       <c r="B32" s="4"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
-      <c r="E32" s="1"/>
       <c r="F32" s="6" t="str">
         <f>IF(ISNUMBER(F31),IF((F31)&gt;SMALL($B$3:$B$6000,1),(F31-1),""),"")</f>
         <v/>
@@ -2293,7 +2517,6 @@
       <c r="B33" s="4"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
-      <c r="E33" s="1"/>
       <c r="F33" s="6" t="str">
         <f>IF(ISNUMBER(F32),IF((F32)&gt;SMALL($B$3:$B$6000,1),(F32-1),""),"")</f>
         <v/>
@@ -2303,7 +2526,6 @@
       <c r="B34" s="4"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
-      <c r="E34" s="1"/>
       <c r="F34" s="6" t="str">
         <f>IF(ISNUMBER(F33),IF((F33)&gt;SMALL($B$3:$B$6000,1),(F33-1),""),"")</f>
         <v/>
@@ -2313,7 +2535,6 @@
       <c r="B35" s="4"/>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
-      <c r="E35" s="1"/>
       <c r="F35" s="6" t="str">
         <f>IF(ISNUMBER(F34),IF((F34)&gt;SMALL($B$3:$B$6000,1),(F34-1),""),"")</f>
         <v/>
@@ -2323,7 +2544,6 @@
       <c r="B36" s="4"/>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
-      <c r="E36" s="1"/>
       <c r="F36" s="6" t="str">
         <f>IF(ISNUMBER(F35),IF((F35)&gt;SMALL($B$3:$B$6000,1),(F35-1),""),"")</f>
         <v/>
@@ -2333,7 +2553,6 @@
       <c r="B37" s="4"/>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
-      <c r="E37" s="1"/>
       <c r="F37" s="6" t="str">
         <f>IF(ISNUMBER(F36),IF((F36)&gt;SMALL($B$3:$B$6000,1),(F36-1),""),"")</f>
         <v/>
@@ -2343,7 +2562,6 @@
       <c r="B38" s="4"/>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
-      <c r="E38" s="1"/>
       <c r="F38" s="6" t="str">
         <f>IF(ISNUMBER(F37),IF((F37)&gt;SMALL($B$3:$B$6000,1),(F37-1),""),"")</f>
         <v/>
@@ -2353,7 +2571,6 @@
       <c r="B39" s="4"/>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
-      <c r="E39" s="1"/>
       <c r="F39" s="6" t="str">
         <f>IF(ISNUMBER(F38),IF((F38)&gt;SMALL($B$3:$B$6000,1),(F38-1),""),"")</f>
         <v/>
@@ -2363,7 +2580,6 @@
       <c r="B40" s="4"/>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
-      <c r="E40" s="1"/>
       <c r="F40" s="6" t="str">
         <f>IF(ISNUMBER(F39),IF((F39)&gt;SMALL($B$3:$B$6000,1),(F39-1),""),"")</f>
         <v/>
@@ -2373,7 +2589,6 @@
       <c r="B41" s="4"/>
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
-      <c r="E41" s="1"/>
       <c r="F41" s="6" t="str">
         <f>IF(ISNUMBER(F40),IF((F40)&gt;SMALL($B$3:$B$6000,1),(F40-1),""),"")</f>
         <v/>
@@ -2383,7 +2598,6 @@
       <c r="B42" s="4"/>
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
-      <c r="E42" s="1"/>
       <c r="F42" s="6" t="str">
         <f>IF(ISNUMBER(F41),IF((F41)&gt;SMALL($B$3:$B$6000,1),(F41-1),""),"")</f>
         <v/>
@@ -2393,7 +2607,6 @@
       <c r="B43" s="4"/>
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
-      <c r="E43" s="1"/>
       <c r="F43" s="6" t="str">
         <f>IF(ISNUMBER(F42),IF((F42)&gt;SMALL($B$3:$B$6000,1),(F42-1),""),"")</f>
         <v/>
@@ -2403,7 +2616,6 @@
       <c r="B44" s="4"/>
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
-      <c r="E44" s="1"/>
       <c r="F44" s="6" t="str">
         <f>IF(ISNUMBER(F43),IF((F43)&gt;SMALL($B$3:$B$6000,1),(F43-1),""),"")</f>
         <v/>
@@ -2413,7 +2625,6 @@
       <c r="B45" s="4"/>
       <c r="C45" s="5"/>
       <c r="D45" s="5"/>
-      <c r="E45" s="1"/>
       <c r="F45" s="6" t="str">
         <f>IF(ISNUMBER(F44),IF((F44)&gt;SMALL($B$3:$B$6000,1),(F44-1),""),"")</f>
         <v/>
@@ -2423,7 +2634,6 @@
       <c r="B46" s="4"/>
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
-      <c r="E46" s="1"/>
       <c r="F46" s="6" t="str">
         <f>IF(ISNUMBER(F45),IF((F45)&gt;SMALL($B$3:$B$6000,1),(F45-1),""),"")</f>
         <v/>
@@ -2433,7 +2643,6 @@
       <c r="B47" s="4"/>
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
-      <c r="E47" s="1"/>
       <c r="F47" s="6" t="str">
         <f>IF(ISNUMBER(F46),IF((F46)&gt;SMALL($B$3:$B$6000,1),(F46-1),""),"")</f>
         <v/>
@@ -2443,7 +2652,6 @@
       <c r="B48" s="4"/>
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
-      <c r="E48" s="1"/>
       <c r="F48" s="6" t="str">
         <f>IF(ISNUMBER(F47),IF((F47)&gt;SMALL($B$3:$B$6000,1),(F47-1),""),"")</f>
         <v/>
@@ -2453,7 +2661,6 @@
       <c r="B49" s="4"/>
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
-      <c r="E49" s="1"/>
       <c r="F49" s="6" t="str">
         <f>IF(ISNUMBER(F48),IF((F48)&gt;SMALL($B$3:$B$6000,1),(F48-1),""),"")</f>
         <v/>
@@ -2463,7 +2670,6 @@
       <c r="B50" s="4"/>
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
-      <c r="E50" s="1"/>
       <c r="F50" s="6" t="str">
         <f>IF(ISNUMBER(F49),IF((F49)&gt;SMALL($B$3:$B$6000,1),(F49-1),""),"")</f>
         <v/>
@@ -2473,7 +2679,6 @@
       <c r="B51" s="4"/>
       <c r="C51" s="5"/>
       <c r="D51" s="5"/>
-      <c r="E51" s="1"/>
       <c r="F51" s="6" t="str">
         <f>IF(ISNUMBER(F50),IF((F50)&gt;SMALL($B$3:$B$6000,1),(F50-1),""),"")</f>
         <v/>
@@ -2483,7 +2688,6 @@
       <c r="B52" s="4"/>
       <c r="C52" s="5"/>
       <c r="D52" s="5"/>
-      <c r="E52" s="1"/>
       <c r="F52" s="6" t="str">
         <f>IF(ISNUMBER(F51),IF((F51)&gt;SMALL($B$3:$B$6000,1),(F51-1),""),"")</f>
         <v/>
@@ -2493,7 +2697,6 @@
       <c r="B53" s="4"/>
       <c r="C53" s="5"/>
       <c r="D53" s="5"/>
-      <c r="E53" s="1"/>
       <c r="F53" s="6" t="str">
         <f>IF(ISNUMBER(F52),IF((F52)&gt;SMALL($B$3:$B$6000,1),(F52-1),""),"")</f>
         <v/>
@@ -2503,7 +2706,6 @@
       <c r="B54" s="4"/>
       <c r="C54" s="5"/>
       <c r="D54" s="5"/>
-      <c r="E54" s="1"/>
       <c r="F54" s="6" t="str">
         <f>IF(ISNUMBER(F53),IF((F53)&gt;SMALL($B$3:$B$6000,1),(F53-1),""),"")</f>
         <v/>
@@ -2513,7 +2715,6 @@
       <c r="B55" s="4"/>
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
-      <c r="E55" s="1"/>
       <c r="F55" s="6" t="str">
         <f>IF(ISNUMBER(F54),IF((F54)&gt;SMALL($B$3:$B$6000,1),(F54-1),""),"")</f>
         <v/>
@@ -2523,7 +2724,6 @@
       <c r="B56" s="4"/>
       <c r="C56" s="5"/>
       <c r="D56" s="5"/>
-      <c r="E56" s="1"/>
       <c r="F56" s="6" t="str">
         <f>IF(ISNUMBER(F55),IF((F55)&gt;SMALL($B$3:$B$6000,1),(F55-1),""),"")</f>
         <v/>
@@ -2533,7 +2733,6 @@
       <c r="B57" s="4"/>
       <c r="C57" s="5"/>
       <c r="D57" s="5"/>
-      <c r="E57" s="1"/>
       <c r="F57" s="6" t="str">
         <f>IF(ISNUMBER(F56),IF((F56)&gt;SMALL($B$3:$B$6000,1),(F56-1),""),"")</f>
         <v/>
@@ -2543,7 +2742,6 @@
       <c r="B58" s="4"/>
       <c r="C58" s="5"/>
       <c r="D58" s="5"/>
-      <c r="E58" s="1"/>
       <c r="F58" s="6" t="str">
         <f>IF(ISNUMBER(F57),IF((F57)&gt;SMALL($B$3:$B$6000,1),(F57-1),""),"")</f>
         <v/>
@@ -2553,7 +2751,6 @@
       <c r="B59" s="4"/>
       <c r="C59" s="5"/>
       <c r="D59" s="5"/>
-      <c r="E59" s="1"/>
       <c r="F59" s="6" t="str">
         <f>IF(ISNUMBER(F58),IF((F58)&gt;SMALL($B$3:$B$6000,1),(F58-1),""),"")</f>
         <v/>
@@ -2563,7 +2760,6 @@
       <c r="B60" s="4"/>
       <c r="C60" s="5"/>
       <c r="D60" s="5"/>
-      <c r="E60" s="1"/>
       <c r="F60" s="6" t="str">
         <f>IF(ISNUMBER(F59),IF((F59)&gt;SMALL($B$3:$B$6000,1),(F59-1),""),"")</f>
         <v/>

</xml_diff>